<commit_message>
Add constant gases that was missed
</commit_message>
<xml_diff>
--- a/tests/modern_sulfur_cycle/settings.xlsx
+++ b/tests/modern_sulfur_cycle/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1221e7247ec036c5/学术会议/25_10_31 PATMO workshop/modern sulfur cycle/input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{1BD0B8D4-4172-A941-A55C-4E1980980DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21BB58E3-CA9F-4D0D-A1EA-A200B89EB2D0}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{1BD0B8D4-4172-A941-A55C-4E1980980DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D326EB62-BA9F-4C9E-9BC6-ED4A1786F517}"/>
   <bookViews>
-    <workbookView xWindow="21075" yWindow="1140" windowWidth="15375" windowHeight="19080" xr2:uid="{06C37378-65EC-8349-A749-809AD85E710E}"/>
+    <workbookView xWindow="12690" yWindow="1500" windowWidth="16410" windowHeight="18975" xr2:uid="{06C37378-65EC-8349-A749-809AD85E710E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>cellsNumber</t>
   </si>
@@ -99,10 +99,6 @@
     <t>molecule/cm3/s (put # if no input)</t>
   </si>
   <si>
-    <t>#constant_species</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>emission_species</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -147,6 +143,14 @@
   </si>
   <si>
     <t>useWaterRemoval</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>constant_species</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">HO2, N, CO2, H2O, CO, O2, N2, OH, O, H2, H, O3, </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -154,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,12 +187,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,7 +210,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -223,9 +221,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8537C3E-DE4A-A54B-9562-BA16146EEF99}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -606,7 +601,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3">
         <v>1000</v>
@@ -658,7 +653,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -691,7 +686,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -702,7 +697,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -713,44 +708,46 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>